<commit_message>
add Q Read to Excell
</commit_message>
<xml_diff>
--- a/src/resources/ÜlkelerTest.xlsx
+++ b/src/resources/ÜlkelerTest.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/IdeaProjects/tryToIt/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC849F56-92C0-3A4F-941B-AD40255188E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DEFE17-36CB-534F-B757-0DB926C8CC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" activeTab="1" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$264</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="626">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1914,6 +1915,9 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>BBB</t>
   </si>
 </sst>
 </file>
@@ -2298,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0230EFE-D68B-AB44-86B3-2FCA054EA626}">
   <dimension ref="A1:D264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5775,5 +5779,97 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC08476-4D72-D349-A2DF-EBB82D0B1090}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add q read Excel
</commit_message>
<xml_diff>
--- a/src/resources/ÜlkelerTest.xlsx
+++ b/src/resources/ÜlkelerTest.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/IdeaProjects/tryToIt/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DEFE17-36CB-534F-B757-0DB926C8CC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D129C-405D-8444-B964-47903634ED43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" activeTab="1" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$264</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="A">Sheet1!$JDY$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="626">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -2302,8 +2303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0230EFE-D68B-AB44-86B3-2FCA054EA626}">
   <dimension ref="A1:D264"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="111" workbookViewId="0">
+      <selection activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2330,6 +2331,15 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -2545,6 +2555,15 @@
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -2802,6 +2821,15 @@
       <c r="A37" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -3115,6 +3143,15 @@
       <c r="A60" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="B60" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -3176,6 +3213,15 @@
       <c r="A65" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="B65" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -3293,6 +3339,15 @@
       <c r="A74" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="B74" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -3410,6 +3465,15 @@
       <c r="A83" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="B83" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
@@ -3625,6 +3689,15 @@
       <c r="A99" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="100" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
@@ -3700,6 +3773,15 @@
       <c r="A105" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="B105" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="106" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
@@ -3831,6 +3913,15 @@
       <c r="A115" s="1" t="s">
         <v>296</v>
       </c>
+      <c r="B115" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="116" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
@@ -3878,6 +3969,15 @@
       <c r="A119" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="B119" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="120" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -4003,6 +4103,15 @@
       <c r="A129" s="1" t="s">
         <v>329</v>
       </c>
+      <c r="B129" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="130" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -4134,6 +4243,15 @@
       <c r="A139" s="1" t="s">
         <v>351</v>
       </c>
+      <c r="B139" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="140" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
@@ -4447,6 +4565,15 @@
       <c r="A162" s="1" t="s">
         <v>401</v>
       </c>
+      <c r="B162" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="163" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
@@ -4648,6 +4775,15 @@
       <c r="A177" s="1" t="s">
         <v>433</v>
       </c>
+      <c r="B177" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="178" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
@@ -4667,6 +4803,15 @@
       <c r="A179" s="1" t="s">
         <v>437</v>
       </c>
+      <c r="B179" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="180" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
@@ -4840,6 +4985,15 @@
       <c r="A192" s="1" t="s">
         <v>463</v>
       </c>
+      <c r="B192" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="193" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
@@ -4859,6 +5013,15 @@
       <c r="A194" s="1" t="s">
         <v>466</v>
       </c>
+      <c r="B194" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="195" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
@@ -4920,6 +5083,15 @@
       <c r="A199" s="1" t="s">
         <v>476</v>
       </c>
+      <c r="B199" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="200" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
@@ -5289,6 +5461,15 @@
       <c r="A226" s="1" t="s">
         <v>539</v>
       </c>
+      <c r="B226" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="227" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
@@ -5504,6 +5685,15 @@
       <c r="A242" s="1" t="s">
         <v>577</v>
       </c>
+      <c r="B242" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="243" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
@@ -5607,6 +5797,15 @@
       <c r="A250" s="1" t="s">
         <v>595</v>
       </c>
+      <c r="B250" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>595</v>
+      </c>
     </row>
     <row r="251" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
@@ -5696,6 +5895,15 @@
       <c r="A257" s="1" t="s">
         <v>607</v>
       </c>
+      <c r="B257" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="258" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
@@ -5729,6 +5937,15 @@
       <c r="A260" s="1" t="s">
         <v>613</v>
       </c>
+      <c r="B260" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="261" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
@@ -5748,6 +5965,15 @@
       <c r="A262" s="1" t="s">
         <v>617</v>
       </c>
+      <c r="B262" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="263" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
@@ -5778,6 +6004,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{C0230EFE-D68B-AB44-86B3-2FCA054EA626}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5787,7 +6014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC08476-4D72-D349-A2DF-EBB82D0B1090}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add to write to excell
</commit_message>
<xml_diff>
--- a/src/resources/ÜlkelerTest.xlsx
+++ b/src/resources/ÜlkelerTest.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/IdeaProjects/tryToIt/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D129C-405D-8444-B964-47903634ED43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF673332-5BC5-AE41-9A1B-F40D52E8A089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="630">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1919,12 +1919,25 @@
   </si>
   <si>
     <t>BBB</t>
+  </si>
+  <si>
+    <t>Nüfus</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>54000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2301,16 +2314,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0230EFE-D68B-AB44-86B3-2FCA054EA626}">
-  <dimension ref="A1:D264"/>
+  <dimension ref="A1:O264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="111" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="28" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="4" customWidth="true" style="1" width="28.0"/>
+    <col min="5" max="16384" style="1" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -2326,6 +2339,9 @@
       <c r="D1" s="1" t="s">
         <v>621</v>
       </c>
+      <c r="E1" t="s" s="1">
+        <v>626</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2340,6 +2356,15 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s" s="1">
+        <v>627</v>
+      </c>
+      <c r="J2" t="s" s="1">
+        <v>628</v>
+      </c>
+      <c r="O2" t="s" s="1">
+        <v>629</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -2452,6 +2477,9 @@
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E10" t="s" s="1">
+        <v>628</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -2522,6 +2550,9 @@
       <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E15" t="n" s="1">
+        <v>54000.0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -6004,7 +6035,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{C0230EFE-D68B-AB44-86B3-2FCA054EA626}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -6020,7 +6050,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="24.5" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" width="24.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add Raed Excell QuestionÂ
</commit_message>
<xml_diff>
--- a/src/resources/ÜlkelerTest.xlsx
+++ b/src/resources/ÜlkelerTest.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafa/IdeaProjects/tryToIt/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C51CFAC-ADC8-0345-A2BE-6F2C4DBB1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9234C5AB-2BCD-9F4A-8C15-B86EB3AEA915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{0976802D-C02C-8D45-8DCC-3701F60D933A}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1934,7 +1934,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2314,13 +2313,13 @@
   <dimension ref="A1:O264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" customWidth="true" style="1" width="28.0"/>
-    <col min="5" max="16384" style="1" width="10.83203125"/>
+    <col min="1" max="4" width="28" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -2385,6 +2384,9 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6044,7 +6046,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" customWidth="true" width="24.5"/>
+    <col min="1" max="5" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>